<commit_message>
Day 11 problem done.
</commit_message>
<xml_diff>
--- a/Love Babber sheet DSA.xlsx
+++ b/Love Babber sheet DSA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1838,7 +1838,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2386,7 +2386,9 @@
       <c r="C16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>465</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>

</xml_diff>